<commit_message>
organizando dados do fabricius, e no futuro espero welington
</commit_message>
<xml_diff>
--- a/dados/brutos/welington_cladosamarali_hemipenis.xlsx
+++ b/dados/brutos/welington_cladosamarali_hemipenis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Welington/Dropbox/Wellington_LACV/DISSERTAÇÃO/Planilhas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55655b1a8b6da948/Documentos/mestrado_unb/lacv/analises_mestrado/dados/brutos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C638BF-F949-864A-B5F9-8E87198B3E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{11C638BF-F949-864A-B5F9-8E87198B3E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BCB1263-DFF1-4DBE-9517-ABDFEC9B9C73}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FAF03B8A-FCE3-AF40-B138-DA6E36832BC7}"/>
+    <workbookView xWindow="8300" yWindow="-50" windowWidth="8780" windowHeight="10800" xr2:uid="{FAF03B8A-FCE3-AF40-B138-DA6E36832BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Espécie</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>CHUNB 37088</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,7 +222,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -518,17 +521,17 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.375" customWidth="1"/>
-    <col min="2" max="2" width="13.875" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.875" style="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -554,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -587,7 +590,7 @@
         <v>0.57299843014128726</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -620,7 +623,7 @@
         <v>0.48111227701993708</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -653,7 +656,7 @@
         <v>0.45184568415209542</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -686,7 +689,7 @@
         <v>0.58695652173913049</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -719,7 +722,7 @@
         <v>0.6010280743376829</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -752,7 +755,7 @@
         <v>0.56781609195402305</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -785,7 +788,7 @@
         <v>0.52907854984894254</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -818,7 +821,7 @@
         <v>0.60068931560807481</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -851,7 +854,7 @@
         <v>0.46040942448821937</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -884,7 +887,7 @@
         <v>0.48493068113321275</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -917,37 +920,40 @@
         <v>0.65208065208065213</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>

</xml_diff>

<commit_message>
finalmente o megazord ta completo
</commit_message>
<xml_diff>
--- a/dados/brutos/welington_cladosamarali_hemipenis.xlsx
+++ b/dados/brutos/welington_cladosamarali_hemipenis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55655b1a8b6da948/Documentos/mestrado_unb/lacv/analises_mestrado/dados/brutos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{11C638BF-F949-864A-B5F9-8E87198B3E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BCB1263-DFF1-4DBE-9517-ABDFEC9B9C73}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{11C638BF-F949-864A-B5F9-8E87198B3E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B2F235-7657-4B81-83D9-7C7906184E0A}"/>
   <bookViews>
-    <workbookView xWindow="8300" yWindow="-50" windowWidth="8780" windowHeight="10800" xr2:uid="{FAF03B8A-FCE3-AF40-B138-DA6E36832BC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FAF03B8A-FCE3-AF40-B138-DA6E36832BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Espécie</t>
   </si>
@@ -65,70 +65,49 @@
     <t>Gymnodactylus darwinii</t>
   </si>
   <si>
-    <t>MTR 12450</t>
-  </si>
-  <si>
     <t>Gymnodactylus sp1</t>
   </si>
   <si>
-    <t>MTR 16143</t>
-  </si>
-  <si>
     <t>Gymnodactylus sp2</t>
   </si>
   <si>
-    <t>UFMG 01327</t>
-  </si>
-  <si>
     <t>Gymnodactylus sp3</t>
   </si>
   <si>
-    <t>UFMG 02175</t>
-  </si>
-  <si>
     <t>Gymnodactylus geckoides</t>
   </si>
   <si>
-    <t>LACV 3288</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado B</t>
   </si>
   <si>
-    <t>LACV 03236</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado C</t>
   </si>
   <si>
-    <t>CHUNB 67393</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado D</t>
   </si>
   <si>
-    <t>CHUNB 00832</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado E</t>
   </si>
   <si>
-    <t>CHUNB 63198</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado F</t>
   </si>
   <si>
-    <t>CHUNB 11514</t>
-  </si>
-  <si>
     <t>Gymnodactylus Clado G</t>
   </si>
   <si>
-    <t>CHUNB 37088</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>MTR</t>
+  </si>
+  <si>
+    <t>UFMG</t>
+  </si>
+  <si>
+    <t>LACV</t>
+  </si>
+  <si>
+    <t>CHUNB</t>
+  </si>
+  <si>
+    <t>Colecao</t>
   </si>
 </sst>
 </file>
@@ -219,6 +198,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,445 +501,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65C05A-05DB-7041-829F-F5DF792C0944}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12450</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.548</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4.46</v>
+      </c>
+      <c r="G2" s="4">
+        <f>E2/D2</f>
+        <v>1.7452054794520548</v>
+      </c>
+      <c r="H2" s="5">
+        <f>D2/F2</f>
+        <v>0.3273542600896861</v>
+      </c>
+      <c r="I2" s="5">
+        <f>E2/F2</f>
+        <v>0.57130044843049332</v>
+      </c>
+      <c r="J2" s="6">
+        <f>D2/E2</f>
+        <v>0.57299843014128726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
-        <v>1.46</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2.548</v>
-      </c>
-      <c r="E2" s="3">
-        <v>4.46</v>
-      </c>
-      <c r="F2" s="4">
-        <f>D2/C2</f>
-        <v>1.7452054794520548</v>
-      </c>
-      <c r="G2" s="5">
-        <f>C2/E2</f>
-        <v>0.3273542600896861</v>
-      </c>
-      <c r="H2" s="5">
-        <f>D2/E2</f>
-        <v>0.57130044843049332</v>
-      </c>
-      <c r="I2" s="6">
-        <f>C2/D2</f>
-        <v>0.57299843014128726</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>16143</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.8340000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.8119999999999998</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6.5650000000000004</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G12" si="0">E3/D3</f>
+        <v>2.0785169029443837</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H12" si="1">D3/F3</f>
+        <v>0.27936024371667934</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I12" si="2">E3/F3</f>
+        <v>0.58065498857578057</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J12" si="3">D3/E3</f>
+        <v>0.48111227701993708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.8340000000000001</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3.8119999999999998</v>
-      </c>
-      <c r="E3" s="3">
-        <v>6.5650000000000004</v>
-      </c>
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F12" si="0">D3/C3</f>
-        <v>2.0785169029443837</v>
-      </c>
-      <c r="G3" s="5">
-        <f t="shared" ref="G3:G12" si="1">C3/E3</f>
-        <v>0.27936024371667934</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H12" si="2">D3/E3</f>
-        <v>0.58065498857578057</v>
-      </c>
-      <c r="I3" s="6">
-        <f t="shared" ref="I3:I12" si="3">C3/D3</f>
-        <v>0.48111227701993708</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1327</v>
+      </c>
+      <c r="D4" s="3">
         <v>1.6279999999999999</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>3.6030000000000002</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>6.024</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <f t="shared" si="0"/>
         <v>2.2131449631449636</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <f t="shared" si="1"/>
         <v>0.27025232403718458</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <f t="shared" si="2"/>
         <v>0.59810756972111556</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <f t="shared" si="3"/>
         <v>0.45184568415209542</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2175</v>
+      </c>
+      <c r="D5" s="3">
         <v>1.2150000000000001</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>2.0699999999999998</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>3.617</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>1.7037037037037035</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <f t="shared" si="1"/>
         <v>0.33591374066906277</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <f t="shared" si="2"/>
         <v>0.57229748410284764</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <f t="shared" si="3"/>
         <v>0.58695652173913049</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3288</v>
+      </c>
+      <c r="D6" s="3">
         <v>1.52</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>2.5289999999999999</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>3.7189999999999999</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>1.663815789473684</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <f t="shared" si="1"/>
         <v>0.40871201936004303</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <f t="shared" si="2"/>
         <v>0.68002151115891374</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <f t="shared" si="3"/>
         <v>0.6010280743376829</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3236</v>
+      </c>
+      <c r="D7" s="3">
         <v>1.7290000000000001</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>3.0449999999999999</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>4.8769999999999998</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>1.7611336032388663</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <f t="shared" si="1"/>
         <v>0.3545212220627435</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <f t="shared" si="2"/>
         <v>0.62435923723600573</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <f t="shared" si="3"/>
         <v>0.56781609195402305</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>67393</v>
+      </c>
+      <c r="D8" s="3">
         <v>1.401</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>2.6480000000000001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>3.9449999999999998</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>1.8900785153461814</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>0.35513307984790876</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <f t="shared" si="2"/>
         <v>0.67122940430925226</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <f t="shared" si="3"/>
         <v>0.52907854984894254</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
+        <v>832</v>
+      </c>
+      <c r="D9" s="3">
         <v>1.22</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>2.0310000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>4.0540000000000003</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>1.6647540983606559</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>0.30093734583127774</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <f t="shared" si="2"/>
         <v>0.50098667982239764</v>
       </c>
-      <c r="I9" s="6">
+      <c r="J9" s="6">
         <f t="shared" si="3"/>
         <v>0.60068931560807481</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1">
+        <v>63198</v>
+      </c>
+      <c r="D10" s="3">
         <v>1.1919999999999999</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>2.589</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>4.3289999999999997</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>2.1719798657718123</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <f t="shared" si="1"/>
         <v>0.27535227535227536</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <f t="shared" si="2"/>
         <v>0.59805959805959807</v>
       </c>
-      <c r="I10" s="6">
+      <c r="J10" s="6">
         <f t="shared" si="3"/>
         <v>0.46040942448821937</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11514</v>
+      </c>
+      <c r="D11" s="3">
         <v>1.609</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>3.3180000000000001</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>5.2229999999999999</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>2.0621504039776259</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <f t="shared" si="1"/>
         <v>0.30806050162741722</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <f t="shared" si="2"/>
         <v>0.63526708788052844</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <f t="shared" si="3"/>
         <v>0.48493068113321275</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <v>37088</v>
+      </c>
+      <c r="D12" s="3">
         <v>1.52</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>2.331</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>3.3290000000000002</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>1.5335526315789474</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="5">
         <f t="shared" si="1"/>
         <v>0.45659357164313608</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <f t="shared" si="2"/>
         <v>0.7002102733553619</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <f t="shared" si="3"/>
         <v>0.65208065208065213</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C14" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C15" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C16" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>